<commit_message>
WIP: data from excel file
</commit_message>
<xml_diff>
--- a/public/static/excel/test.xlsx
+++ b/public/static/excel/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Pulpit\Next.js\index-generator\index-generator\public\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB39F00-07AA-49AF-922F-39D562733E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9CE11E-163B-4FCB-A6A7-FE8B53A8FDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>dupa</t>
+  </si>
+  <si>
+    <t>legia</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>chuje</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>lech</t>
+  </si>
+  <si>
+    <t>mistrz</t>
+  </si>
+  <si>
+    <t>polski</t>
   </si>
 </sst>
 </file>
@@ -345,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -358,6 +379,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WIP: reading datta from excel file
</commit_message>
<xml_diff>
--- a/public/static/excel/test.xlsx
+++ b/public/static/excel/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Pulpit\Next.js\index-generator\index-generator\public\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9CE11E-163B-4FCB-A6A7-FE8B53A8FDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1427A6-07F2-4A9A-B66F-B340B9E30554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,30 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>dupa</t>
-  </si>
-  <si>
-    <t>legia</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>chuje</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>lech</t>
-  </si>
-  <si>
-    <t>mistrz</t>
-  </si>
-  <si>
-    <t>polski</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>12.9</t>
+  </si>
+  <si>
+    <t>A2-70</t>
+  </si>
+  <si>
+    <t>A4-70</t>
+  </si>
+  <si>
+    <t>A4-80</t>
+  </si>
+  <si>
+    <t>S235</t>
+  </si>
+  <si>
+    <t>S275</t>
+  </si>
+  <si>
+    <t>S355</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>DH36</t>
+  </si>
+  <si>
+    <t>EH36</t>
+  </si>
+  <si>
+    <t>1.4404</t>
+  </si>
+  <si>
+    <t>1.4362</t>
+  </si>
+  <si>
+    <t>42CrMo4</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>B7</t>
   </si>
 </sst>
 </file>
@@ -84,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -366,52 +400,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>